<commit_message>
time series part 1
</commit_message>
<xml_diff>
--- a/tests/modules/orcaflex/orcaflex_post_process/results/opp_summary1.xlsx
+++ b/tests/modules/orcaflex/orcaflex_post_process/results/opp_summary1.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>.\orcaflex_test1.sim</t>
+          <t>k:\github\digitalmodel\tests\modules\orcaflex\orcaflex_post_process\orcaflex_test1.sim</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -531,7 +531,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>.\orcaflex_test1.sim</t>
+          <t>k:\github\digitalmodel\tests\modules\orcaflex\orcaflex_post_process\orcaflex_test1.sim</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -578,7 +578,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>.\orcaflex_test2.sim</t>
+          <t>k:\github\digitalmodel\tests\modules\orcaflex\orcaflex_post_process\orcaflex_test2.sim</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -588,7 +588,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>.\orcaflex_test2.sim</t>
+          <t>k:\github\digitalmodel\tests\modules\orcaflex\orcaflex_post_process\orcaflex_test2.sim</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">

</xml_diff>

<commit_message>
orcaflex tests with refactor
</commit_message>
<xml_diff>
--- a/tests/modules/orcaflex/orcaflex_post_process/results/opp_summary1.xlsx
+++ b/tests/modules/orcaflex/orcaflex_post_process/results/opp_summary1.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>k:\github\digitalmodel\tests\modules\orcaflex\orcaflex_post_process\orcaflex_test1.sim</t>
+          <t>k:/github/digitalmodel/tests/modules/orcaflex/orcaflex_post_process/orcaflex_test1.sim</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -531,7 +531,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>k:\github\digitalmodel\tests\modules\orcaflex\orcaflex_post_process\orcaflex_test1.sim</t>
+          <t>k:/github/digitalmodel/tests/modules/orcaflex/orcaflex_post_process/orcaflex_test1.sim</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -578,7 +578,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>k:\github\digitalmodel\tests\modules\orcaflex\orcaflex_post_process\orcaflex_test2.sim</t>
+          <t>k:/github/digitalmodel/tests/modules/orcaflex/orcaflex_post_process/orcaflex_test2.sim</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -588,7 +588,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>k:\github\digitalmodel\tests\modules\orcaflex\orcaflex_post_process\orcaflex_test2.sim</t>
+          <t>k:/github/digitalmodel/tests/modules/orcaflex/orcaflex_post_process/orcaflex_test2.sim</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">

</xml_diff>